<commit_message>
page de suppression des données terminés
</commit_message>
<xml_diff>
--- a/todo-list/todo.xlsx
+++ b/todo-list/todo.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Page web" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>A faire</t>
   </si>
@@ -73,13 +73,67 @@
   </si>
   <si>
     <t>8h-40</t>
+  </si>
+  <si>
+    <t>Contenu</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Un bouton pour Réinitialiser les données</t>
+  </si>
+  <si>
+    <t>Formulaire pour faire l'importation</t>
+  </si>
+  <si>
+    <t>Un dropdown pour choisir le nom de la table</t>
+  </si>
+  <si>
+    <t>Un dropdown pour choisir le separateur</t>
+  </si>
+  <si>
+    <t>Un inputu de type file pour télversé le fichier csv</t>
+  </si>
+  <si>
+    <t>Un lien pour reinitialisér les données sauf les users</t>
+  </si>
+  <si>
+    <t>Un PopUp de confirmation du suppression</t>
+  </si>
+  <si>
+    <t>10min</t>
+  </si>
+  <si>
+    <t>5min</t>
+  </si>
+  <si>
+    <t>18min</t>
+  </si>
+  <si>
+    <t>Fonctionnalité</t>
+  </si>
+  <si>
+    <t>METETIER</t>
+  </si>
+  <si>
+    <t>PAGES</t>
+  </si>
+  <si>
+    <t>Crée une fonction pour supprimer les données</t>
+  </si>
+  <si>
+    <t>Supprimer les données sauf les users</t>
+  </si>
+  <si>
+    <t>deb-13h30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,8 +141,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,8 +197,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -154,11 +238,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -167,7 +341,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -175,11 +348,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,106 +713,225 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E1" s="1" t="s">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="5"/>
-      <c r="F2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E3" s="2"/>
-      <c r="F3" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="35"/>
+    </row>
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="6" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fonction delete data terminé
</commit_message>
<xml_diff>
--- a/todo-list/todo.xlsx
+++ b/todo-list/todo.xlsx
@@ -126,7 +126,7 @@
     <t>Supprimer les données sauf les users</t>
   </si>
   <si>
-    <t>deb-13h30</t>
+    <t>1h33</t>
   </si>
 </sst>
 </file>
@@ -349,89 +349,89 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,24 +716,24 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -750,116 +750,116 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
-      <c r="C4" s="35"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="21"/>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="9" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="16"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="7"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="16"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="4"/>
       <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="16"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="16"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="4"/>
       <c r="E9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="3"/>
       <c r="E10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="14" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="20" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="15" t="s">
+      <c r="A14" s="34"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="4"/>
@@ -868,11 +868,11 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="4"/>
@@ -881,9 +881,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="16" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="14" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="4"/>
@@ -892,9 +892,9 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="16" t="s">
+      <c r="A17" s="35"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="4"/>
@@ -903,22 +903,22 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="4"/>
       <c r="E18" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="16" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creation d'une customerCsv comme modele
</commit_message>
<xml_diff>
--- a/todo-list/todo.xlsx
+++ b/todo-list/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>A faire</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>1h23</t>
+  </si>
+  <si>
+    <t>Création d'une class model pour l'import</t>
+  </si>
+  <si>
+    <t>Une class pour mapper les nom de colonnes dans le fichier csv</t>
+  </si>
+  <si>
+    <t>21min</t>
   </si>
 </sst>
 </file>
@@ -716,7 +725,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,6 +926,17 @@
         <v>35</v>
       </c>
     </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Modification du todo list pour marquer l'importation customer terminé
</commit_message>
<xml_diff>
--- a/todo-list/todo.xlsx
+++ b/todo-list/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>A faire</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>21min</t>
+  </si>
+  <si>
+    <t>1h31</t>
+  </si>
+  <si>
+    <t>Crée une fonction pour upload un fichier csv pour la table customer</t>
   </si>
 </sst>
 </file>
@@ -341,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -391,15 +397,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -440,6 +446,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -724,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +775,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
-      <c r="C4" s="21"/>
+      <c r="C4" s="20"/>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
@@ -861,7 +876,7 @@
         <v>25</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="19" t="s">
         <v>27</v>
       </c>
     </row>
@@ -912,29 +927,42 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="5" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -943,7 +971,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A18:A20"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D12:E12"/>

</xml_diff>

<commit_message>
fonction generer user, customer et ticket terminé sans test
</commit_message>
<xml_diff>
--- a/todo-list/todo.xlsx
+++ b/todo-list/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>A faire</t>
   </si>
@@ -39,9 +39,6 @@
     <t>1h30</t>
   </si>
   <si>
-    <t>Réinitialiser les données de la base</t>
-  </si>
-  <si>
     <t>Import csv</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>11h11</t>
   </si>
   <si>
-    <t>8h-40</t>
-  </si>
-  <si>
     <t>Contenu</t>
   </si>
   <si>
@@ -142,6 +136,15 @@
   </si>
   <si>
     <t>Crée une fonction pour upload un fichier csv pour la table customer</t>
+  </si>
+  <si>
+    <t>Generation données</t>
+  </si>
+  <si>
+    <t>Crée une fonction pour generer des données pour un Entité donnée</t>
+  </si>
+  <si>
+    <t>Génerer des données de test pour un table donnée</t>
   </si>
 </sst>
 </file>
@@ -181,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,8 +221,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -257,50 +266,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -343,11 +308,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -355,7 +331,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -376,9 +351,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -406,57 +378,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,245 +710,332 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="17" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
-      <c r="C4" s="20"/>
-    </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="8" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E6" s="35" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="4"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B13" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="C15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="D18" s="3"/>
+      <c r="E18" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="37"/>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="37"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="31"/>
+      <c r="B24" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5" t="s">
+      <c r="D24" s="37"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="31"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="21" t="s">
+      <c r="B27" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>14</v>
-      </c>
+      <c r="C27" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="37"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B26"/>
     <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A12:E12"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A13:A17"/>

</xml_diff>

<commit_message>
generation des données il n'y pas de teste mais on commence la partie 2
</commit_message>
<xml_diff>
--- a/todo-list/todo.xlsx
+++ b/todo-list/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>A faire</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Génerer des données de test pour un table donnée</t>
+  </si>
+  <si>
+    <t>Comprehension du projet actuel</t>
+  </si>
+  <si>
+    <t>9H03</t>
   </si>
 </sst>
 </file>
@@ -323,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -384,6 +390,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -393,43 +409,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,28 +760,28 @@
       <c r="C4" s="18"/>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="24" t="s">
         <v>2</v>
       </c>
     </row>
@@ -830,59 +839,59 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B14" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="17" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="11" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>20</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="27"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="38" t="s">
+        <v>19</v>
+      </c>
       <c r="C16" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4" t="s">
@@ -890,10 +899,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4" t="s">
@@ -901,144 +910,155 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>31</v>
-      </c>
+      <c r="A18" s="35"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="12" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>29</v>
+      </c>
       <c r="B19" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="12"/>
+        <v>34</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="D20" s="3"/>
       <c r="E20" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
+    <row r="22" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B23" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="37"/>
-      <c r="E22" s="20"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="11" t="s">
+      <c r="D23" s="25"/>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="27" t="s">
+      <c r="D24" s="25"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
+      <c r="B25" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="12" t="s">
+      <c r="D25" s="25"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="12" t="s">
+      <c r="D26" s="25"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="35"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="D27" s="25"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B28" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C28" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="37"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="21"/>
       <c r="C29" s="12"/>
-      <c r="D29" s="37"/>
+      <c r="D29" s="25"/>
       <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A22:E22"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A14:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modification de MCD en ajoutant la table budget et depense
</commit_message>
<xml_diff>
--- a/todo-list/todo.xlsx
+++ b/todo-list/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>A faire</t>
   </si>
@@ -144,13 +144,34 @@
     <t>Crée une fonction pour generer des données pour un Entité donnée</t>
   </si>
   <si>
-    <t>Génerer des données de test pour un table donnée</t>
-  </si>
-  <si>
     <t>Comprehension du projet actuel</t>
   </si>
   <si>
     <t>9H03</t>
+  </si>
+  <si>
+    <t>Gestion de budget et depense</t>
+  </si>
+  <si>
+    <t>Formulaire pour choisir la  table pour generer les données</t>
+  </si>
+  <si>
+    <t>BASE DE DONNEE</t>
+  </si>
+  <si>
+    <t>Crée une table pour stocker le budget rattacher à un client</t>
+  </si>
+  <si>
+    <t>Crée une table pour stocker le depense rattacher à un ticket et un lead</t>
+  </si>
+  <si>
+    <t>2h 29min</t>
+  </si>
+  <si>
+    <t>Crée les class pour representer la table budget et depense</t>
+  </si>
+  <si>
+    <t>11h20</t>
   </si>
 </sst>
 </file>
@@ -329,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -400,6 +421,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -438,6 +462,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,13 +796,13 @@
       <c r="C4" s="18"/>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
     </row>
     <row r="6" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
@@ -785,7 +821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
@@ -795,7 +831,7 @@
       <c r="E7" s="4"/>
       <c r="G7" s="13"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>3</v>
       </c>
@@ -806,7 +842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
@@ -817,7 +853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>4</v>
       </c>
@@ -828,7 +864,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
@@ -839,31 +875,31 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="22"/>
       <c r="C12" s="12"/>
       <c r="D12" s="2"/>
       <c r="E12" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -874,9 +910,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="37"/>
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="11" t="s">
         <v>24</v>
       </c>
@@ -885,9 +921,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="38" t="s">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="39" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="12" t="s">
@@ -898,9 +934,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="38"/>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
@@ -909,9 +945,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="38"/>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="12" t="s">
         <v>22</v>
       </c>
@@ -920,8 +956,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="19" t="s">
@@ -935,8 +971,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+    <row r="20" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
       <c r="B20" s="19" t="s">
         <v>34</v>
       </c>
@@ -948,8 +984,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
+    <row r="21" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="29"/>
       <c r="B21" s="19" t="s">
         <v>38</v>
       </c>
@@ -959,95 +995,190 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+    <row r="22" spans="1:5" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+    </row>
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="C23" s="12"/>
       <c r="D23" s="25"/>
       <c r="E23" s="20"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="11" t="s">
-        <v>24</v>
-      </c>
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
+      <c r="B24" s="38"/>
       <c r="D24" s="25"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>20</v>
-      </c>
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="35"/>
+      <c r="B25" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="12"/>
       <c r="D25" s="25"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="12" t="s">
-        <v>21</v>
-      </c>
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="35"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="25"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="12" t="s">
-        <v>22</v>
-      </c>
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="36"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="25"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
+    <row r="28" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="C28" s="12"/>
       <c r="D28" s="25"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
       <c r="B29" s="21"/>
       <c r="C29" s="12"/>
       <c r="D29" s="25"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="29"/>
       <c r="B30" s="21"/>
       <c r="C30" s="12"/>
       <c r="D30" s="25"/>
       <c r="E30" s="4"/>
     </row>
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="20"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="35"/>
+      <c r="B33" s="38"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="35"/>
+      <c r="B34" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="35"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="36"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="29"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="43"/>
+      <c r="B41" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="41"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="18">
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="A37:A39"/>
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A22:E22"/>
     <mergeCell ref="A5:E5"/>

</xml_diff>